<commit_message>
Se arregla el exportar informes tanto en txt y en excel, se mojoran los informes.
</commit_message>
<xml_diff>
--- a/errores.xlsx
+++ b/errores.xlsx
@@ -473,18 +473,21 @@
     <t>89. Costo anual de incapacidades laborales relacionadas con la AR</t>
   </si>
   <si>
-    <t>RES00</t>
+    <t>SAP035</t>
   </si>
   <si>
     <t>E</t>
   </si>
   <si>
+    <t xml:space="preserve"> jose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdhfsjh </t>
+  </si>
+  <si>
     <t>NONE</t>
   </si>
   <si>
-    <t xml:space="preserve">sdhfsjh </t>
-  </si>
-  <si>
     <t>CC</t>
   </si>
   <si>
@@ -495,9 +498,6 @@
   </si>
   <si>
     <t>70001</t>
-  </si>
-  <si>
-    <t>r</t>
   </si>
   <si>
     <t>050010412701</t>
@@ -1336,7 +1336,7 @@
         <v>153</v>
       </c>
       <c r="C2" t="n">
-        <v>99</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
         <v>154</v>
@@ -1345,34 +1345,34 @@
         <v>155</v>
       </c>
       <c r="F2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I2" t="n">
         <v>34534643</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>28446</v>
+        <v>31693</v>
       </c>
       <c r="K2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="L2" t="n">
         <v>6</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>158</v>
+      <c r="M2" t="s">
+        <v>159</v>
       </c>
       <c r="N2" t="n">
         <v>3145747676</v>
       </c>
       <c r="O2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="P2" s="2" t="n">
         <v>36935</v>
@@ -1416,8 +1416,8 @@
       <c r="AC2" t="n">
         <v>0</v>
       </c>
-      <c r="AD2" t="n">
-        <v>300</v>
+      <c r="AD2" s="3" t="n">
+        <v>301</v>
       </c>
       <c r="AE2" t="n">
         <v>0</v>
@@ -1470,8 +1470,8 @@
       <c r="AU2" t="n">
         <v>1</v>
       </c>
-      <c r="AV2" s="3" t="s">
-        <v>160</v>
+      <c r="AV2" t="n">
+        <v>1</v>
       </c>
       <c r="AW2" t="n">
         <v>1</v>
@@ -1612,7 +1612,7 @@
         <v>-36888</v>
       </c>
       <c r="CQ2" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="CR2" t="n">
         <v>6</v>
@@ -1797,19 +1797,19 @@
         <v>99</v>
       </c>
       <c r="D3" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E3" t="s">
         <v>162</v>
       </c>
       <c r="F3" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G3" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I3" t="n">
         <v>34534643</v>
@@ -1818,19 +1818,19 @@
         <v>28446</v>
       </c>
       <c r="K3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="L3" t="n">
         <v>6</v>
       </c>
-      <c r="M3" s="3" t="s">
-        <v>158</v>
+      <c r="M3" t="s">
+        <v>159</v>
       </c>
       <c r="N3" t="n">
         <v>3145747676</v>
       </c>
       <c r="O3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="P3" s="2" t="n">
         <v>36935</v>
@@ -2255,19 +2255,19 @@
         <v>99</v>
       </c>
       <c r="D4" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E4" t="s">
         <v>162</v>
       </c>
       <c r="F4" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G4" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I4" t="n">
         <v>34534643</v>
@@ -2276,19 +2276,19 @@
         <v>28446</v>
       </c>
       <c r="K4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="L4" t="n">
         <v>6</v>
       </c>
-      <c r="M4" s="3" t="s">
-        <v>158</v>
+      <c r="M4" t="s">
+        <v>159</v>
       </c>
       <c r="N4" t="n">
         <v>3145747676</v>
       </c>
       <c r="O4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="P4" s="2" t="n">
         <v>36935</v>

</xml_diff>

<commit_message>
Base del proyecto funcional
</commit_message>
<xml_diff>
--- a/errores.xlsx
+++ b/errores.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="169">
   <si>
     <t>1. Código de la EAPB o de la entidad territorial</t>
   </si>
@@ -476,34 +476,52 @@
     <t>SAP035</t>
   </si>
   <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> jose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdhfsjh </t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>CL 13 CRA 18   17-18 B FLORIDA MAGANGUE</t>
+  </si>
+  <si>
+    <t>25280</t>
+  </si>
+  <si>
+    <t>1799-01-01</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>050010412701</t>
+  </si>
+  <si>
     <t>E</t>
   </si>
   <si>
-    <t xml:space="preserve"> jose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdhfsjh </t>
-  </si>
-  <si>
-    <t>NONE</t>
+    <t>hghgh</t>
   </si>
   <si>
     <t>CC</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>CL 13 CRA 18  # 17-18. B. FLORIDA MAGANGUE</t>
-  </si>
-  <si>
     <t>70001</t>
   </si>
   <si>
-    <t>050010412701</t>
-  </si>
-  <si>
-    <t>hghgh</t>
+    <t>CL 13 CRA 18  17-18  B FLORIDA MAGANGUE</t>
   </si>
 </sst>
 </file>
@@ -511,7 +529,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt formatCode="yyyy-mm-dd" numFmtId="164"/>
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -1377,14 +1395,14 @@
       <c r="P2" s="2" t="n">
         <v>36935</v>
       </c>
-      <c r="Q2" s="2" t="n">
-        <v>-32506</v>
+      <c r="Q2" t="s">
+        <v>161</v>
       </c>
       <c r="R2" s="2" t="n">
         <v>36970</v>
       </c>
-      <c r="S2" s="2" t="n">
-        <v>-36888</v>
+      <c r="S2" t="s">
+        <v>161</v>
       </c>
       <c r="T2" t="n">
         <v>164</v>
@@ -1416,8 +1434,8 @@
       <c r="AC2" t="n">
         <v>0</v>
       </c>
-      <c r="AD2" s="3" t="n">
-        <v>301</v>
+      <c r="AD2" t="n">
+        <v>300</v>
       </c>
       <c r="AE2" t="n">
         <v>0</v>
@@ -1446,8 +1464,8 @@
       <c r="AM2" t="n">
         <v>1</v>
       </c>
-      <c r="AN2" s="2" t="n">
-        <v>-36888</v>
+      <c r="AN2" t="s">
+        <v>161</v>
       </c>
       <c r="AO2" t="n">
         <v>1</v>
@@ -1455,8 +1473,8 @@
       <c r="AP2" t="n">
         <v>300</v>
       </c>
-      <c r="AQ2" s="2" t="n">
-        <v>-36888</v>
+      <c r="AQ2" t="s">
+        <v>161</v>
       </c>
       <c r="AR2" t="n">
         <v>300</v>
@@ -1464,20 +1482,20 @@
       <c r="AS2" s="2" t="n">
         <v>36935</v>
       </c>
-      <c r="AT2" t="n">
-        <v>0</v>
+      <c r="AT2" s="3" t="s">
+        <v>162</v>
       </c>
       <c r="AU2" t="n">
         <v>1</v>
       </c>
-      <c r="AV2" t="n">
-        <v>1</v>
+      <c r="AV2" s="3" t="s">
+        <v>162</v>
       </c>
       <c r="AW2" t="n">
         <v>1</v>
       </c>
-      <c r="AX2" s="2" t="n">
-        <v>-36888</v>
+      <c r="AX2" t="s">
+        <v>161</v>
       </c>
       <c r="AY2" t="n">
         <v>0</v>
@@ -1608,8 +1626,8 @@
       <c r="CO2" t="n">
         <v>1</v>
       </c>
-      <c r="CP2" s="2" t="n">
-        <v>-36888</v>
+      <c r="CP2" t="s">
+        <v>161</v>
       </c>
       <c r="CQ2" t="n">
         <v>1</v>
@@ -1620,8 +1638,8 @@
       <c r="CS2" t="n">
         <v>300</v>
       </c>
-      <c r="CT2" s="2" t="n">
-        <v>-36888</v>
+      <c r="CT2" t="s">
+        <v>161</v>
       </c>
       <c r="CU2" t="n">
         <v>300</v>
@@ -1747,13 +1765,13 @@
         <v>0</v>
       </c>
       <c r="EJ2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="EK2" t="n">
         <v>25148</v>
       </c>
-      <c r="EL2" s="2" t="n">
-        <v>-36888</v>
+      <c r="EL2" t="s">
+        <v>161</v>
       </c>
       <c r="EM2" t="n">
         <v>6</v>
@@ -1761,14 +1779,14 @@
       <c r="EN2" t="n">
         <v>0</v>
       </c>
-      <c r="EO2" s="2" t="n">
-        <v>-36888</v>
-      </c>
-      <c r="EP2" t="n">
-        <v>999999</v>
-      </c>
-      <c r="EQ2" s="2" t="n">
-        <v>-36888</v>
+      <c r="EO2" t="s">
+        <v>161</v>
+      </c>
+      <c r="EP2" t="s">
+        <v>163</v>
+      </c>
+      <c r="EQ2" t="s">
+        <v>161</v>
       </c>
       <c r="ER2" t="n">
         <v>0</v>
@@ -1791,7 +1809,7 @@
         <v>152</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="C3" t="n">
         <v>99</v>
@@ -1800,7 +1818,7 @@
         <v>156</v>
       </c>
       <c r="E3" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="F3" t="s">
         <v>156</v>
@@ -1809,7 +1827,7 @@
         <v>156</v>
       </c>
       <c r="H3" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="I3" t="n">
         <v>34534643</v>
@@ -1830,19 +1848,19 @@
         <v>3145747676</v>
       </c>
       <c r="O3" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="P3" s="2" t="n">
         <v>36935</v>
       </c>
-      <c r="Q3" s="2" t="n">
-        <v>36935</v>
+      <c r="Q3" t="s">
+        <v>161</v>
       </c>
       <c r="R3" s="2" t="n">
         <v>36970</v>
       </c>
-      <c r="S3" s="2" t="n">
-        <v>-36888</v>
+      <c r="S3" t="s">
+        <v>161</v>
       </c>
       <c r="T3" t="n">
         <v>164</v>
@@ -1904,8 +1922,8 @@
       <c r="AM3" t="n">
         <v>1</v>
       </c>
-      <c r="AN3" s="2" t="n">
-        <v>-36888</v>
+      <c r="AN3" t="s">
+        <v>161</v>
       </c>
       <c r="AO3" t="n">
         <v>1</v>
@@ -1913,8 +1931,8 @@
       <c r="AP3" t="n">
         <v>300</v>
       </c>
-      <c r="AQ3" s="2" t="n">
-        <v>-36888</v>
+      <c r="AQ3" t="s">
+        <v>161</v>
       </c>
       <c r="AR3" t="n">
         <v>300</v>
@@ -1934,8 +1952,8 @@
       <c r="AW3" t="n">
         <v>1</v>
       </c>
-      <c r="AX3" s="2" t="n">
-        <v>-36888</v>
+      <c r="AX3" t="s">
+        <v>161</v>
       </c>
       <c r="AY3" t="n">
         <v>0</v>
@@ -2066,8 +2084,8 @@
       <c r="CO3" t="n">
         <v>1</v>
       </c>
-      <c r="CP3" s="2" t="n">
-        <v>-36888</v>
+      <c r="CP3" t="s">
+        <v>161</v>
       </c>
       <c r="CQ3" t="n">
         <v>1</v>
@@ -2078,8 +2096,8 @@
       <c r="CS3" t="n">
         <v>300</v>
       </c>
-      <c r="CT3" s="2" t="n">
-        <v>-36888</v>
+      <c r="CT3" t="s">
+        <v>161</v>
       </c>
       <c r="CU3" t="n">
         <v>300</v>
@@ -2205,13 +2223,13 @@
         <v>0</v>
       </c>
       <c r="EJ3" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="EK3" t="n">
         <v>25148</v>
       </c>
-      <c r="EL3" s="2" t="n">
-        <v>-36888</v>
+      <c r="EL3" t="s">
+        <v>161</v>
       </c>
       <c r="EM3" t="n">
         <v>6</v>
@@ -2219,14 +2237,14 @@
       <c r="EN3" t="n">
         <v>0</v>
       </c>
-      <c r="EO3" s="2" t="n">
-        <v>-36888</v>
-      </c>
-      <c r="EP3" t="n">
-        <v>999999</v>
-      </c>
-      <c r="EQ3" s="2" t="n">
-        <v>-36888</v>
+      <c r="EO3" t="s">
+        <v>161</v>
+      </c>
+      <c r="EP3" t="s">
+        <v>163</v>
+      </c>
+      <c r="EQ3" t="s">
+        <v>161</v>
       </c>
       <c r="ER3" t="n">
         <v>0</v>
@@ -2249,7 +2267,7 @@
         <v>152</v>
       </c>
       <c r="B4" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="C4" t="n">
         <v>99</v>
@@ -2258,7 +2276,7 @@
         <v>156</v>
       </c>
       <c r="E4" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="F4" t="s">
         <v>156</v>
@@ -2267,7 +2285,7 @@
         <v>156</v>
       </c>
       <c r="H4" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="I4" t="n">
         <v>34534643</v>
@@ -2282,25 +2300,25 @@
         <v>6</v>
       </c>
       <c r="M4" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="N4" t="n">
         <v>3145747676</v>
       </c>
       <c r="O4" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="P4" s="2" t="n">
         <v>36935</v>
       </c>
-      <c r="Q4" s="2" t="n">
-        <v>36935</v>
+      <c r="Q4" t="s">
+        <v>161</v>
       </c>
       <c r="R4" s="2" t="n">
         <v>36970</v>
       </c>
-      <c r="S4" s="2" t="n">
-        <v>-36888</v>
+      <c r="S4" t="s">
+        <v>161</v>
       </c>
       <c r="T4" t="n">
         <v>164</v>
@@ -2362,8 +2380,8 @@
       <c r="AM4" t="n">
         <v>1</v>
       </c>
-      <c r="AN4" s="2" t="n">
-        <v>-36888</v>
+      <c r="AN4" t="s">
+        <v>161</v>
       </c>
       <c r="AO4" t="n">
         <v>1</v>
@@ -2371,8 +2389,8 @@
       <c r="AP4" t="n">
         <v>300</v>
       </c>
-      <c r="AQ4" s="2" t="n">
-        <v>-36888</v>
+      <c r="AQ4" t="s">
+        <v>161</v>
       </c>
       <c r="AR4" t="n">
         <v>300</v>
@@ -2392,8 +2410,8 @@
       <c r="AW4" t="n">
         <v>1</v>
       </c>
-      <c r="AX4" s="2" t="n">
-        <v>-36888</v>
+      <c r="AX4" t="s">
+        <v>161</v>
       </c>
       <c r="AY4" t="n">
         <v>0</v>
@@ -2524,8 +2542,8 @@
       <c r="CO4" t="n">
         <v>1</v>
       </c>
-      <c r="CP4" s="2" t="n">
-        <v>-36888</v>
+      <c r="CP4" t="s">
+        <v>161</v>
       </c>
       <c r="CQ4" t="n">
         <v>1</v>
@@ -2536,8 +2554,8 @@
       <c r="CS4" t="n">
         <v>300</v>
       </c>
-      <c r="CT4" s="2" t="n">
-        <v>-36888</v>
+      <c r="CT4" t="s">
+        <v>161</v>
       </c>
       <c r="CU4" t="n">
         <v>300</v>
@@ -2663,13 +2681,13 @@
         <v>0</v>
       </c>
       <c r="EJ4" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="EK4" t="n">
         <v>25148</v>
       </c>
-      <c r="EL4" s="2" t="n">
-        <v>-36888</v>
+      <c r="EL4" t="s">
+        <v>161</v>
       </c>
       <c r="EM4" t="n">
         <v>6</v>
@@ -2677,14 +2695,14 @@
       <c r="EN4" t="n">
         <v>0</v>
       </c>
-      <c r="EO4" s="2" t="n">
-        <v>-36888</v>
+      <c r="EO4" t="s">
+        <v>161</v>
       </c>
       <c r="EP4" t="n">
         <v>999999</v>
       </c>
-      <c r="EQ4" s="2" t="n">
-        <v>-36888</v>
+      <c r="EQ4" t="s">
+        <v>161</v>
       </c>
       <c r="ER4" t="n">
         <v>0</v>

</xml_diff>